<commit_message>
changes after user tesing
</commit_message>
<xml_diff>
--- a/Progress.Diary.xlsx
+++ b/Progress.Diary.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
   <si>
     <t>Progress Diary</t>
   </si>
@@ -224,7 +224,7 @@
     <t>Week 1</t>
   </si>
   <si>
-    <t>Code von app.py geändert, Lösungen für Token-Problem überlegen, User Testing</t>
+    <t>Code von app.py geändert, Lösungen für Token-Problem überlegen, User Testing vorbereiten</t>
   </si>
   <si>
     <t>Vorbereitung eines Usability Testings.</t>
@@ -239,7 +239,46 @@
     <t>Week 2</t>
   </si>
   <si>
-    <t>User Testing und Auswertung der Tests</t>
+    <t>Landing Page Vorschläge erstellen. User Testing und Auswertung der Tests, Entscheidung für und Priorisierung von nötigen Änderungen/Anpassungen, die die Tests uns gezeigt haben</t>
+  </si>
+  <si>
+    <t>Ein User Testing durchzuführen und im Anschluss auszuwerten.</t>
+  </si>
+  <si>
+    <t>Meinen Vorschlag für eine Landing Page in Firma erstellt. User Test zu Hause lokal durchgeführt.</t>
+  </si>
+  <si>
+    <t>Die Erstellung meines Landing Page Vorschlags hat mir großen Spaß gemacht. Es ist gar nicht so einfach, ein User Testing allein durchzuführen, da man Moderator, Beobachter und Protokollant in einem ist.</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Entscheidung für die Landing Page treffen. Abschlusspräsentation vorbereiten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurz gefasst alle wichtigen Informationen und Learnings des Projektes in eine Präsentation verpacken. </t>
+  </si>
+  <si>
+    <t>Landing Page Vorschläge aller zu einem finalen Konzept zusammengefasst. Anteilige Mitarbeit an den Präsentationsfolien, Vorbereitung des Chatbot-Demonstration-Teils der Abschlusspräsentation.</t>
+  </si>
+  <si>
+    <t>Durch die Vereinigung unserer Ideen haben wir eine tolle Landing Page gestaltet. Es ist nicht leicht, die Arbeit der letzten Wochen in einer kurzen Präsentation zusammen zu fassen.</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Finalisierung von Sprint2</t>
+  </si>
+  <si>
+    <t>Leider konnte ich keine Lösung finden, wie das Updaten einzelner Blocks durch die Auswahl der Radio Buttons getriggert werden kann.</t>
+  </si>
+  <si>
+    <t>Nach wiederholt fehlgeschlagenem Versuch die Modusauswahl zum Laufen zu bringen, Entscheidung für Weglassen der Modi getroffen. Modusauswahl entfernt. Kleinere Anpassungen am Styling vorgenommen.  Fehlende Inhalte im Wiki ergänzt.</t>
+  </si>
+  <si>
+    <t>Bei unserem Chatbot handelt es sich noch immer um einen Prototyp. Bis zu einem fertigen Produkt wäre noch ein weiter Weg. Ich bin stolz wie weit wir gekommen sind.</t>
   </si>
 </sst>
 </file>
@@ -325,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -346,30 +385,6 @@
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -449,17 +464,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="11"/>
       </left>
       <right style="thin">
@@ -488,26 +492,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -520,110 +511,95 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1710,7 +1686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1718,8 +1694,8 @@
   <cols>
     <col min="1" max="1" width="45.6719" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.6719" style="1" customWidth="1"/>
-    <col min="3" max="5" width="23.3516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="23.3516" style="1" customWidth="1"/>
+    <col min="3" max="4" width="23.3516" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="23.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -1729,738 +1705,833 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="6"/>
     </row>
     <row r="3" ht="14.55" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" t="s" s="8">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" ht="39.45" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="A4" t="s" s="8">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" t="s" s="9">
         <v>3</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" ht="14.55" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" t="s" s="14">
+      <c r="A5" s="11"/>
+      <c r="B5" t="s" s="12">
         <v>4</v>
       </c>
-      <c r="C5" t="s" s="14">
+      <c r="C5" t="s" s="12">
         <v>5</v>
       </c>
-      <c r="D5" t="s" s="14">
+      <c r="D5" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="E5" s="15"/>
     </row>
     <row r="6" ht="63.75" customHeight="1">
-      <c r="A6" t="s" s="10">
+      <c r="A6" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="B6" t="s" s="16">
+      <c r="B6" t="s" s="13">
         <v>8</v>
       </c>
-      <c r="C6" t="s" s="16">
+      <c r="C6" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="D6" t="s" s="16">
+      <c r="D6" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="E6" s="15"/>
     </row>
     <row r="7" ht="184.8" customHeight="1">
-      <c r="A7" t="s" s="10">
+      <c r="A7" t="s" s="8">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="16">
+      <c r="B7" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="C7" t="s" s="17">
+      <c r="C7" t="s" s="14">
         <v>13</v>
       </c>
-      <c r="D7" t="s" s="17">
+      <c r="D7" t="s" s="14">
         <v>14</v>
       </c>
-      <c r="E7" s="15"/>
     </row>
     <row r="8" ht="14.55" customHeight="1">
-      <c r="A8" t="s" s="10">
+      <c r="A8" t="s" s="8">
         <v>15</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="15">
         <v>600</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="15">
         <v>450</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="15">
         <v>500</v>
       </c>
-      <c r="E8" s="15"/>
     </row>
     <row r="9" ht="42" customHeight="1">
-      <c r="A9" t="s" s="10">
+      <c r="A9" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="B9" t="s" s="17">
+      <c r="B9" t="s" s="14">
         <v>17</v>
       </c>
-      <c r="C9" t="s" s="17">
+      <c r="C9" t="s" s="14">
         <v>18</v>
       </c>
-      <c r="D9" t="s" s="17">
+      <c r="D9" t="s" s="14">
         <v>19</v>
       </c>
-      <c r="E9" s="15"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" ht="14.55" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" t="s" s="8">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s" s="6">
         <v>20</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" ht="26.55" customHeight="1">
-      <c r="A12" t="s" s="21">
+      <c r="A12" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="B12" t="s" s="22">
+      <c r="B12" t="s" s="19">
         <v>21</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" ht="14.55" customHeight="1">
-      <c r="A13" s="24"/>
-      <c r="B13" t="s" s="25">
+      <c r="A13" s="21"/>
+      <c r="B13" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="C13" t="s" s="25">
+      <c r="C13" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="D13" t="s" s="25">
+      <c r="D13" t="s" s="22">
         <v>6</v>
       </c>
-      <c r="E13" s="15"/>
     </row>
     <row r="14" ht="110.4" customHeight="1">
-      <c r="A14" t="s" s="21">
+      <c r="A14" t="s" s="18">
         <v>7</v>
       </c>
-      <c r="B14" t="s" s="26">
+      <c r="B14" t="s" s="23">
         <v>23</v>
       </c>
-      <c r="C14" t="s" s="26">
+      <c r="C14" t="s" s="23">
         <v>24</v>
       </c>
-      <c r="D14" t="s" s="26">
+      <c r="D14" t="s" s="23">
         <v>25</v>
       </c>
-      <c r="E14" s="15"/>
     </row>
     <row r="15" ht="220.8" customHeight="1">
-      <c r="A15" t="s" s="21">
+      <c r="A15" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="B15" t="s" s="26">
+      <c r="B15" t="s" s="23">
         <v>26</v>
       </c>
-      <c r="C15" t="s" s="26">
+      <c r="C15" t="s" s="23">
         <v>27</v>
       </c>
-      <c r="D15" t="s" s="26">
+      <c r="D15" t="s" s="23">
         <v>28</v>
       </c>
-      <c r="E15" s="15"/>
     </row>
     <row r="16" ht="14.55" customHeight="1">
-      <c r="A16" t="s" s="21">
+      <c r="A16" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="24">
         <v>420</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="24">
         <v>200</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="24">
         <v>200</v>
       </c>
-      <c r="E16" s="15"/>
     </row>
     <row r="17" ht="110.4" customHeight="1">
-      <c r="A17" t="s" s="21">
+      <c r="A17" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="26">
+      <c r="B17" t="s" s="23">
         <v>29</v>
       </c>
-      <c r="C17" t="s" s="26">
+      <c r="C17" t="s" s="23">
         <v>30</v>
       </c>
-      <c r="D17" t="s" s="26">
+      <c r="D17" t="s" s="23">
         <v>31</v>
       </c>
-      <c r="E17" s="15"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="6"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
     </row>
     <row r="19" ht="14.55" customHeight="1">
-      <c r="A19" s="30"/>
-      <c r="B19" t="s" s="31">
+      <c r="A19" s="27"/>
+      <c r="B19" t="s" s="28">
         <v>32</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="6"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
     </row>
     <row r="20" ht="14.55" customHeight="1">
-      <c r="A20" t="s" s="21">
+      <c r="A20" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="B20" t="s" s="33">
+      <c r="B20" t="s" s="30">
         <v>33</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
     </row>
     <row r="21" ht="14.55" customHeight="1">
-      <c r="A21" s="24"/>
-      <c r="B21" t="s" s="25">
+      <c r="A21" s="21"/>
+      <c r="B21" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="C21" t="s" s="25">
+      <c r="C21" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="D21" t="s" s="25">
+      <c r="D21" t="s" s="22">
         <v>6</v>
       </c>
-      <c r="E21" s="15"/>
     </row>
     <row r="22" ht="165.6" customHeight="1">
-      <c r="A22" t="s" s="21">
+      <c r="A22" t="s" s="18">
         <v>7</v>
       </c>
-      <c r="B22" t="s" s="26">
+      <c r="B22" t="s" s="23">
         <v>34</v>
       </c>
-      <c r="C22" t="s" s="26">
+      <c r="C22" t="s" s="23">
         <v>35</v>
       </c>
-      <c r="D22" t="s" s="26">
+      <c r="D22" t="s" s="23">
         <v>36</v>
       </c>
-      <c r="E22" s="15"/>
     </row>
     <row r="23" ht="138" customHeight="1">
-      <c r="A23" t="s" s="21">
+      <c r="A23" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="B23" t="s" s="26">
+      <c r="B23" t="s" s="23">
         <v>37</v>
       </c>
-      <c r="C23" t="s" s="26">
+      <c r="C23" t="s" s="23">
         <v>38</v>
       </c>
-      <c r="D23" t="s" s="26">
+      <c r="D23" t="s" s="23">
         <v>39</v>
       </c>
-      <c r="E23" s="15"/>
     </row>
     <row r="24" ht="14.55" customHeight="1">
-      <c r="A24" t="s" s="21">
+      <c r="A24" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="24">
         <v>330</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C24" s="24">
         <v>500</v>
       </c>
-      <c r="D24" s="27">
+      <c r="D24" s="24">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" ht="220.8" customHeight="1">
+      <c r="A25" t="s" s="18">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s" s="23">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s" s="23">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s" s="23">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" ht="14.55" customHeight="1">
+      <c r="A27" s="27"/>
+      <c r="B27" t="s" s="28">
+        <v>43</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+    </row>
+    <row r="28" ht="38.55" customHeight="1">
+      <c r="A28" t="s" s="18">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s" s="19">
+        <v>44</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" ht="14.55" customHeight="1">
+      <c r="A29" s="21"/>
+      <c r="B29" t="s" s="22">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s" s="22">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" ht="193.2" customHeight="1">
+      <c r="A30" t="s" s="18">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s" s="23">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s" s="23">
+        <v>46</v>
+      </c>
+      <c r="D30" t="s" s="23">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" ht="193.2" customHeight="1">
+      <c r="A31" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s" s="23">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s" s="23">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s" s="23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" ht="14.55" customHeight="1">
+      <c r="A32" t="s" s="18">
+        <v>15</v>
+      </c>
+      <c r="B32" s="24">
+        <v>600</v>
+      </c>
+      <c r="C32" s="24">
+        <v>600</v>
+      </c>
+      <c r="D32" s="24">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" ht="96.6" customHeight="1">
+      <c r="A33" t="s" s="18">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s" s="23">
+        <v>51</v>
+      </c>
+      <c r="C33" t="s" s="23">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s" s="23">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" ht="13.5" customHeight="1">
+      <c r="A34" s="31"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+    </row>
+    <row r="35" ht="14.55" customHeight="1">
+      <c r="A35" s="31"/>
+      <c r="B35" t="s" s="28">
+        <v>54</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+    </row>
+    <row r="36" ht="14.6" customHeight="1">
+      <c r="A36" t="s" s="18">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s" s="19">
+        <v>55</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+    </row>
+    <row r="37" ht="14.55" customHeight="1">
+      <c r="A37" s="21"/>
+      <c r="B37" t="s" s="22">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s" s="22">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" ht="86.6" customHeight="1">
+      <c r="A38" t="s" s="18">
+        <v>7</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" t="s" s="23">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" ht="62.6" customHeight="1">
+      <c r="A39" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" t="s" s="23">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" ht="14.55" customHeight="1">
+      <c r="A40" t="s" s="18">
+        <v>15</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="24">
         <v>120</v>
       </c>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" ht="220.8" customHeight="1">
-      <c r="A25" t="s" s="21">
+    </row>
+    <row r="41" ht="26.6" customHeight="1">
+      <c r="A41" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="B25" t="s" s="26">
-        <v>40</v>
-      </c>
-      <c r="C25" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="D25" t="s" s="26">
-        <v>42</v>
-      </c>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" ht="14.55" customHeight="1">
-      <c r="A27" s="30"/>
-      <c r="B27" t="s" s="31">
-        <v>43</v>
-      </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" ht="38.55" customHeight="1">
-      <c r="A28" t="s" s="21">
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" t="s" s="23">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" ht="13.5" customHeight="1">
+      <c r="A42" s="31"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+    </row>
+    <row r="43" ht="14.55" customHeight="1">
+      <c r="A43" s="31"/>
+      <c r="B43" t="s" s="28">
+        <v>59</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+    </row>
+    <row r="44" ht="14.6" customHeight="1">
+      <c r="A44" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="B28" t="s" s="22">
-        <v>44</v>
-      </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" ht="14.55" customHeight="1">
-      <c r="A29" s="24"/>
-      <c r="B29" t="s" s="25">
+      <c r="B44" t="s" s="19">
+        <v>60</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+    </row>
+    <row r="45" ht="14.55" customHeight="1">
+      <c r="A45" s="21"/>
+      <c r="B45" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="C29" t="s" s="25">
+      <c r="C45" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="D29" t="s" s="25">
+      <c r="D45" t="s" s="22">
         <v>6</v>
       </c>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" ht="193.2" customHeight="1">
-      <c r="A30" t="s" s="21">
+    </row>
+    <row r="46" ht="110.6" customHeight="1">
+      <c r="A46" t="s" s="18">
         <v>7</v>
       </c>
-      <c r="B30" t="s" s="26">
-        <v>45</v>
-      </c>
-      <c r="C30" t="s" s="26">
-        <v>46</v>
-      </c>
-      <c r="D30" t="s" s="26">
-        <v>47</v>
-      </c>
-      <c r="E30" s="15"/>
-    </row>
-    <row r="31" ht="193.2" customHeight="1">
-      <c r="A31" t="s" s="21">
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" t="s" s="23">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" ht="74.6" customHeight="1">
+      <c r="A47" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="B31" t="s" s="26">
-        <v>48</v>
-      </c>
-      <c r="C31" t="s" s="26">
-        <v>49</v>
-      </c>
-      <c r="D31" t="s" s="26">
-        <v>50</v>
-      </c>
-      <c r="E31" s="15"/>
-    </row>
-    <row r="32" ht="14.55" customHeight="1">
-      <c r="A32" t="s" s="21">
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" t="s" s="23">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" ht="14.55" customHeight="1">
+      <c r="A48" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="B32" s="27">
-        <v>600</v>
-      </c>
-      <c r="C32" s="27">
-        <v>600</v>
-      </c>
-      <c r="D32" s="27">
-        <v>600</v>
-      </c>
-      <c r="E32" s="15"/>
-    </row>
-    <row r="33" ht="96.6" customHeight="1">
-      <c r="A33" t="s" s="21">
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" ht="50.6" customHeight="1">
+      <c r="A49" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="B33" t="s" s="26">
-        <v>51</v>
-      </c>
-      <c r="C33" t="s" s="26">
-        <v>52</v>
-      </c>
-      <c r="D33" t="s" s="26">
-        <v>53</v>
-      </c>
-      <c r="E33" s="15"/>
-    </row>
-    <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="34"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" ht="14.55" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" t="s" s="31">
-        <v>54</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" ht="14.6" customHeight="1">
-      <c r="A36" t="s" s="21">
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" t="s" s="23">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" ht="14.55" customHeight="1">
+      <c r="A50" s="18"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+    </row>
+    <row r="51" ht="14.55" customHeight="1">
+      <c r="A51" s="31"/>
+      <c r="B51" t="s" s="28">
+        <v>64</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+    </row>
+    <row r="52" ht="26.6" customHeight="1">
+      <c r="A52" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="B36" t="s" s="22">
-        <v>55</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" ht="14.55" customHeight="1">
-      <c r="A37" s="24"/>
-      <c r="B37" t="s" s="25">
+      <c r="B52" t="s" s="19">
+        <v>65</v>
+      </c>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+    </row>
+    <row r="53" ht="14.55" customHeight="1">
+      <c r="A53" s="21"/>
+      <c r="B53" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="C37" t="s" s="25">
+      <c r="C53" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="D37" t="s" s="25">
+      <c r="D53" t="s" s="22">
         <v>6</v>
       </c>
-      <c r="E37" s="15"/>
-    </row>
-    <row r="38" ht="86.6" customHeight="1">
-      <c r="A38" t="s" s="21">
+    </row>
+    <row r="54" ht="26.6" customHeight="1">
+      <c r="A54" t="s" s="18">
         <v>7</v>
       </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" t="s" s="26">
-        <v>56</v>
-      </c>
-      <c r="E38" s="15"/>
-    </row>
-    <row r="39" ht="62.6" customHeight="1">
-      <c r="A39" t="s" s="21">
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" t="s" s="23">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" ht="98.6" customHeight="1">
+      <c r="A55" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="D39" t="s" s="26">
-        <v>57</v>
-      </c>
-      <c r="E39" s="15"/>
-    </row>
-    <row r="40" ht="14.55" customHeight="1">
-      <c r="A40" t="s" s="21">
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
+      <c r="D55" t="s" s="23">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" ht="14.55" customHeight="1">
+      <c r="A56" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="27">
-        <v>60</v>
-      </c>
-      <c r="E40" s="15"/>
-    </row>
-    <row r="41" ht="26.6" customHeight="1">
-      <c r="A41" t="s" s="21">
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="24">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="57" ht="98.6" customHeight="1">
+      <c r="A57" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" t="s" s="26">
-        <v>58</v>
-      </c>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="34"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" ht="14.55" customHeight="1">
-      <c r="A43" s="34"/>
-      <c r="B43" t="s" s="31">
-        <v>59</v>
-      </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" ht="14.6" customHeight="1">
-      <c r="A44" t="s" s="21">
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" t="s" s="23">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" ht="14.55" customHeight="1">
+      <c r="A58" s="18"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+    </row>
+    <row r="59" ht="14.55" customHeight="1">
+      <c r="A59" s="31"/>
+      <c r="B59" t="s" s="28">
+        <v>69</v>
+      </c>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+    </row>
+    <row r="60" ht="38.6" customHeight="1">
+      <c r="A60" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="B44" t="s" s="22">
-        <v>60</v>
-      </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" ht="14.55" customHeight="1">
-      <c r="A45" s="24"/>
-      <c r="B45" t="s" s="25">
+      <c r="B60" t="s" s="19">
+        <v>70</v>
+      </c>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+    </row>
+    <row r="61" ht="14.55" customHeight="1">
+      <c r="A61" s="21"/>
+      <c r="B61" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="C45" t="s" s="25">
+      <c r="C61" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="D45" t="s" s="25">
+      <c r="D61" t="s" s="22">
         <v>6</v>
       </c>
-      <c r="E45" s="15"/>
-    </row>
-    <row r="46" ht="110.6" customHeight="1">
-      <c r="A46" t="s" s="21">
+    </row>
+    <row r="62" ht="38.6" customHeight="1">
+      <c r="A62" t="s" s="18">
         <v>7</v>
       </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" t="s" s="26">
-        <v>61</v>
-      </c>
-      <c r="E46" s="15"/>
-    </row>
-    <row r="47" ht="74.6" customHeight="1">
-      <c r="A47" t="s" s="21">
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="D62" t="s" s="23">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" ht="50.6" customHeight="1">
+      <c r="A63" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" t="s" s="26">
-        <v>62</v>
-      </c>
-      <c r="E47" s="15"/>
-    </row>
-    <row r="48" ht="14.55" customHeight="1">
-      <c r="A48" t="s" s="21">
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" t="s" s="23">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" ht="14.55" customHeight="1">
+      <c r="A64" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="27">
-        <v>60</v>
-      </c>
-      <c r="E48" s="15"/>
-    </row>
-    <row r="49" ht="50.6" customHeight="1">
-      <c r="A49" t="s" s="21">
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="65" ht="110.6" customHeight="1">
+      <c r="A65" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
-      <c r="D49" t="s" s="26">
-        <v>63</v>
-      </c>
-      <c r="E49" s="15"/>
-    </row>
-    <row r="50" ht="14.55" customHeight="1">
-      <c r="A50" s="21"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="15"/>
-    </row>
-    <row r="51" ht="14.55" customHeight="1">
-      <c r="A51" s="34"/>
-      <c r="B51" t="s" s="31">
-        <v>64</v>
-      </c>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" ht="14.6" customHeight="1">
-      <c r="A52" t="s" s="21">
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" t="s" s="23">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" ht="14.55" customHeight="1">
+      <c r="A66" s="18"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="33"/>
+    </row>
+    <row r="67" ht="14.55" customHeight="1">
+      <c r="A67" s="31"/>
+      <c r="B67" t="s" s="28">
+        <v>74</v>
+      </c>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+    </row>
+    <row r="68" ht="14.55" customHeight="1">
+      <c r="A68" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="B52" t="s" s="22">
-        <v>65</v>
-      </c>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" ht="14.55" customHeight="1">
-      <c r="A53" s="24"/>
-      <c r="B53" t="s" s="25">
+      <c r="B68" t="s" s="19">
+        <v>75</v>
+      </c>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+    </row>
+    <row r="69" ht="14.55" customHeight="1">
+      <c r="A69" s="21"/>
+      <c r="B69" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="C53" t="s" s="25">
+      <c r="C69" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="D53" t="s" s="25">
+      <c r="D69" t="s" s="22">
         <v>6</v>
       </c>
-      <c r="E53" s="15"/>
-    </row>
-    <row r="54" ht="26.6" customHeight="1">
-      <c r="A54" t="s" s="21">
+    </row>
+    <row r="70" ht="62.6" customHeight="1">
+      <c r="A70" t="s" s="18">
         <v>7</v>
       </c>
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
-      <c r="D54" t="s" s="26">
-        <v>66</v>
-      </c>
-      <c r="E54" s="15"/>
-    </row>
-    <row r="55" ht="98.6" customHeight="1">
-      <c r="A55" t="s" s="21">
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
+      <c r="D70" t="s" s="23">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" ht="110.6" customHeight="1">
+      <c r="A71" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35"/>
-      <c r="D55" t="s" s="26">
-        <v>67</v>
-      </c>
-      <c r="E55" s="15"/>
-    </row>
-    <row r="56" ht="14.55" customHeight="1">
-      <c r="A56" t="s" s="21">
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
+      <c r="D71" t="s" s="23">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" ht="14.55" customHeight="1">
+      <c r="A72" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="B56" s="35"/>
-      <c r="C56" s="35"/>
-      <c r="D56" s="27">
-        <v>240</v>
-      </c>
-      <c r="E56" s="15"/>
-    </row>
-    <row r="57" ht="98.6" customHeight="1">
-      <c r="A57" t="s" s="21">
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="24">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="73" ht="98.6" customHeight="1">
+      <c r="A73" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
-      <c r="D57" t="s" s="26">
-        <v>68</v>
-      </c>
-      <c r="E57" s="15"/>
-    </row>
-    <row r="58" ht="14.55" customHeight="1">
-      <c r="A58" s="21"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="15"/>
-    </row>
-    <row r="59" ht="14.55" customHeight="1">
-      <c r="A59" s="34"/>
-      <c r="B59" t="s" s="31">
-        <v>69</v>
-      </c>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="6"/>
-    </row>
-    <row r="60" ht="14.6" customHeight="1">
-      <c r="A60" t="s" s="21">
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
+      <c r="D73" t="s" s="23">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="74" ht="14.55" customHeight="1">
+      <c r="A74" s="18"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="33"/>
+    </row>
+    <row r="75" ht="14.55" customHeight="1">
+      <c r="A75" s="31"/>
+      <c r="B75" t="s" s="28">
+        <v>79</v>
+      </c>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+    </row>
+    <row r="76" ht="14.55" customHeight="1">
+      <c r="A76" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="B60" t="s" s="22">
-        <v>70</v>
-      </c>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" ht="14.55" customHeight="1">
-      <c r="A61" s="24"/>
-      <c r="B61" t="s" s="25">
+      <c r="B76" t="s" s="19">
+        <v>80</v>
+      </c>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+    </row>
+    <row r="77" ht="14.55" customHeight="1">
+      <c r="A77" s="21"/>
+      <c r="B77" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="C61" t="s" s="25">
+      <c r="C77" t="s" s="22">
         <v>22</v>
       </c>
-      <c r="D61" t="s" s="25">
-        <v>22</v>
-      </c>
-      <c r="E61" s="15"/>
-    </row>
-    <row r="62" ht="14.55" customHeight="1">
-      <c r="A62" t="s" s="21">
+      <c r="D77" t="s" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" ht="74.6" customHeight="1">
+      <c r="A78" t="s" s="18">
         <v>7</v>
       </c>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="15"/>
-    </row>
-    <row r="63" ht="14.55" customHeight="1">
-      <c r="A63" t="s" s="21">
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" t="s" s="23">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" ht="134.6" customHeight="1">
+      <c r="A79" t="s" s="18">
         <v>11</v>
       </c>
-      <c r="B63" s="35"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="15"/>
-    </row>
-    <row r="64" ht="14.55" customHeight="1">
-      <c r="A64" t="s" s="21">
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" t="s" s="23">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" ht="14.55" customHeight="1">
+      <c r="A80" t="s" s="18">
         <v>15</v>
       </c>
-      <c r="B64" s="35"/>
-      <c r="C64" s="35"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="15"/>
-    </row>
-    <row r="65" ht="14.55" customHeight="1">
-      <c r="A65" t="s" s="21">
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="24">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="81" ht="86.6" customHeight="1">
+      <c r="A81" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="B65" s="35"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="38"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="32"/>
+      <c r="D81" t="s" s="23">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B20:D20"/>
@@ -2469,6 +2540,8 @@
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B76:D76"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B36" r:id="rId1" location="" tooltip="" display="huggingface.co Space einrichten"/>

</xml_diff>